<commit_message>
CO2 Tax fixed+CO2 tax RampUp defined
</commit_message>
<xml_diff>
--- a/suppxls/Scen_CTax.xlsx
+++ b/suppxls/Scen_CTax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AC2714-E748-4D59-8144-2D9EBAD6456B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65E48DB-B879-4E5A-98B1-4E86E9666F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="1860" windowWidth="26610" windowHeight="13740" activeTab="1" xr2:uid="{7C70B42E-9201-48A9-B8F0-1466C79FDCED}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="26610" windowHeight="13740" activeTab="1" xr2:uid="{7C70B42E-9201-48A9-B8F0-1466C79FDCED}"/>
   </bookViews>
   <sheets>
     <sheet name="CO2TaxInputs" sheetId="5" r:id="rId1"/>
@@ -667,10 +667,10 @@
     <t>Commodity</t>
   </si>
   <si>
-    <t>CO2EQS</t>
+    <t>CO2S</t>
   </si>
   <si>
-    <t>~TFM_INS</t>
+    <t>~TFM_INS-TS</t>
   </si>
 </sst>
 </file>

</xml_diff>